<commit_message>
UPDATE: excel etapas y asignar coordinadores
</commit_message>
<xml_diff>
--- a/excel/Etapas.xlsx
+++ b/excel/Etapas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\php_isa\Incidencias_EVG\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Incidencias_EVG\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -449,7 +449,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -460,7 +460,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -471,7 +471,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>